<commit_message>
Agregado mensaje de alerta al cargar promos invalidas.
</commit_message>
<xml_diff>
--- a/lista_IBMS.xlsx
+++ b/lista_IBMS.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="BUMPS EE" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -48,16 +48,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -426,13 +426,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="50"/>
-    <col customWidth="1" max="5" min="5" width="40"/>
-    <col customWidth="1" max="6" min="6" width="17"/>
-    <col customWidth="1" max="9" min="9" width="10"/>
-    <col customWidth="1" max="10" min="10" width="10"/>
-    <col customWidth="1" max="11" min="11" width="10"/>
-    <col customWidth="1" max="12" min="12" width="15"/>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -627,7 +627,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -645,13 +645,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="50"/>
-    <col customWidth="1" max="5" min="5" width="40"/>
-    <col customWidth="1" max="6" min="6" width="17"/>
-    <col customWidth="1" max="9" min="9" width="10"/>
-    <col customWidth="1" max="10" min="10" width="10"/>
-    <col customWidth="1" max="11" min="11" width="10"/>
-    <col customWidth="1" max="12" min="12" width="15"/>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -760,7 +760,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -778,13 +778,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="50"/>
-    <col customWidth="1" max="5" min="5" width="40"/>
-    <col customWidth="1" max="6" min="6" width="17"/>
-    <col customWidth="1" max="9" min="9" width="10"/>
-    <col customWidth="1" max="10" min="10" width="10"/>
-    <col customWidth="1" max="11" min="11" width="10"/>
-    <col customWidth="1" max="12" min="12" width="15"/>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -809,6 +809,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>